<commit_message>
back to working again lol
</commit_message>
<xml_diff>
--- a/logs/signals.xlsx
+++ b/logs/signals.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R590"/>
+  <dimension ref="A1:R594"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34640,7 +34640,7 @@
         </is>
       </c>
       <c r="B590" s="2" t="n">
-        <v>46027.14330496739</v>
+        <v>46027.14330496528</v>
       </c>
       <c r="C590" t="inlineStr">
         <is>
@@ -34667,11 +34667,7 @@
           <t>REGIME_FILTERED</t>
         </is>
       </c>
-      <c r="H590" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="H590" t="inlineStr"/>
       <c r="I590" t="n">
         <v>0</v>
       </c>
@@ -34695,6 +34691,246 @@
         </is>
       </c>
     </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>S_0590</t>
+        </is>
+      </c>
+      <c r="B591" s="2" t="n">
+        <v>46028.0643036574</v>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>eth-updown-15m-1767663900</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>Ethereum Up or Down - January 5, 8:45PM-9:00PM ET</t>
+        </is>
+      </c>
+      <c r="E591" t="inlineStr">
+        <is>
+          <t>82305470999346288835007647903068954073105635720820601714459832234291951995392</t>
+        </is>
+      </c>
+      <c r="F591" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="G591" t="inlineStr">
+        <is>
+          <t>OVERREACTION</t>
+        </is>
+      </c>
+      <c r="H591" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="I591" t="n">
+        <v>85</v>
+      </c>
+      <c r="J591" t="b">
+        <v>1</v>
+      </c>
+      <c r="K591" t="n">
+        <v>1</v>
+      </c>
+      <c r="L591" t="n">
+        <v>85</v>
+      </c>
+      <c r="M591" t="inlineStr"/>
+      <c r="N591" t="inlineStr"/>
+      <c r="O591" t="inlineStr"/>
+      <c r="P591" t="inlineStr"/>
+      <c r="Q591" t="b">
+        <v>1</v>
+      </c>
+      <c r="R591" t="inlineStr"/>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>S_0591</t>
+        </is>
+      </c>
+      <c r="B592" s="2" t="n">
+        <v>46028.0643119676</v>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>btc-updown-15m-1767663900</t>
+        </is>
+      </c>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>Bitcoin Up or Down - January 5, 8:45PM-9:00PM ET</t>
+        </is>
+      </c>
+      <c r="E592" t="inlineStr">
+        <is>
+          <t>57362101177156983528258207354091914235956383545392935916147920523000585185181</t>
+        </is>
+      </c>
+      <c r="F592" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="G592" t="inlineStr">
+        <is>
+          <t>REGIME_FILTERED</t>
+        </is>
+      </c>
+      <c r="H592" t="inlineStr"/>
+      <c r="I592" t="n">
+        <v>0</v>
+      </c>
+      <c r="J592" t="b">
+        <v>0</v>
+      </c>
+      <c r="K592" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L592" t="inlineStr"/>
+      <c r="M592" t="inlineStr"/>
+      <c r="N592" t="inlineStr"/>
+      <c r="O592" t="inlineStr"/>
+      <c r="P592" t="inlineStr"/>
+      <c r="Q592" t="b">
+        <v>0</v>
+      </c>
+      <c r="R592" t="inlineStr">
+        <is>
+          <t>Failed: Orderbook Balance</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>S_0592</t>
+        </is>
+      </c>
+      <c r="B593" s="2" t="n">
+        <v>46028.06469912037</v>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>eth-updown-15m-1767663900</t>
+        </is>
+      </c>
+      <c r="D593" t="inlineStr">
+        <is>
+          <t>Ethereum Up or Down - January 5, 8:45PM-9:00PM ET</t>
+        </is>
+      </c>
+      <c r="E593" t="inlineStr">
+        <is>
+          <t>82305470999346288835007647903068954073105635720820601714459832234291951995392</t>
+        </is>
+      </c>
+      <c r="F593" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="G593" t="inlineStr">
+        <is>
+          <t>OVERREACTION</t>
+        </is>
+      </c>
+      <c r="H593" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="I593" t="n">
+        <v>85</v>
+      </c>
+      <c r="J593" t="b">
+        <v>1</v>
+      </c>
+      <c r="K593" t="n">
+        <v>1</v>
+      </c>
+      <c r="L593" t="n">
+        <v>85</v>
+      </c>
+      <c r="M593" t="inlineStr"/>
+      <c r="N593" t="inlineStr"/>
+      <c r="O593" t="inlineStr"/>
+      <c r="P593" t="inlineStr"/>
+      <c r="Q593" t="b">
+        <v>1</v>
+      </c>
+      <c r="R593" t="inlineStr"/>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>S_0593</t>
+        </is>
+      </c>
+      <c r="B594" s="2" t="n">
+        <v>46028.06470791745</v>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>btc-updown-15m-1767663900</t>
+        </is>
+      </c>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>Bitcoin Up or Down - January 5, 8:45PM-9:00PM ET</t>
+        </is>
+      </c>
+      <c r="E594" t="inlineStr">
+        <is>
+          <t>57362101177156983528258207354091914235956383545392935916147920523000585185181</t>
+        </is>
+      </c>
+      <c r="F594" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="G594" t="inlineStr">
+        <is>
+          <t>REGIME_FILTERED</t>
+        </is>
+      </c>
+      <c r="H594" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I594" t="n">
+        <v>0</v>
+      </c>
+      <c r="J594" t="b">
+        <v>0</v>
+      </c>
+      <c r="K594" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L594" t="inlineStr"/>
+      <c r="M594" t="inlineStr"/>
+      <c r="N594" t="inlineStr"/>
+      <c r="O594" t="inlineStr"/>
+      <c r="P594" t="inlineStr"/>
+      <c r="Q594" t="b">
+        <v>0</v>
+      </c>
+      <c r="R594" t="inlineStr">
+        <is>
+          <t>Failed: Orderbook Balance</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>